<commit_message>
update by mads po and reports. update by gian, finance and clearance
</commit_message>
<xml_diff>
--- a/do-not-delete-this/admin/reports/excel/template.xlsx
+++ b/do-not-delete-this/admin/reports/excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indang.gov.ph\do-not-delete-this\admin\reports\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2290CDC1-A221-4F8E-ACFA-7F8A400CFBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1DB1D5-5141-4439-8FB3-51696AB8C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9975" yWindow="3615" windowWidth="12315" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL-Resident-report" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -568,10 +568,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -583,6 +579,13 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -942,12 +945,12 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -962,143 +965,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>